<commit_message>
Dodane logowanie bez email i bez hasła
</commit_message>
<xml_diff>
--- a/Dokumentacja.xlsx
+++ b/Dokumentacja.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0DDE82-1DAE-4977-91B5-7DE2CEFE3494}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="2400" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="2400" windowWidth="21600" windowHeight="11505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Nazwa testu</t>
   </si>
@@ -78,13 +77,25 @@
   </si>
   <si>
     <t>Rejestracja użytkownika - prawidłowe dane</t>
+  </si>
+  <si>
+    <t>Login 4</t>
+  </si>
+  <si>
+    <t>Login 5</t>
+  </si>
+  <si>
+    <t>Próba logowania bez wpisania email</t>
+  </si>
+  <si>
+    <t>Próba logowania bez wpisania hasła</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +109,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,12 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -380,28 +397,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela3" displayName="Tabela3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:E6"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nazwa testu" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Opis" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Autor" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Uwagi" dataDxfId="7"/>
+    <tableColumn id="1" name="Nazwa testu" dataDxfId="11"/>
+    <tableColumn id="2" name="Opis" dataDxfId="10"/>
+    <tableColumn id="3" name="Autor" dataDxfId="9"/>
+    <tableColumn id="4" name="Status" dataDxfId="8"/>
+    <tableColumn id="5" name="Uwagi" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela38" displayName="Tabela38" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela38" displayName="Tabela38" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nazwa testu" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Opis" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Autor" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Uwagi" dataDxfId="0"/>
+    <tableColumn id="1" name="Nazwa testu" dataDxfId="4"/>
+    <tableColumn id="2" name="Opis" dataDxfId="3"/>
+    <tableColumn id="3" name="Autor" dataDxfId="2"/>
+    <tableColumn id="4" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" name="Uwagi" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,11 +686,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,94 +837,6 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="52.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
Dokończenie rejestracji i dokumentacja
</commit_message>
<xml_diff>
--- a/Dokumentacja.xlsx
+++ b/Dokumentacja.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E94368-3200-48B3-9075-25395AA5F3B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="2400" windowWidth="21600" windowHeight="11505" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Nazwa testu</t>
   </si>
@@ -89,12 +90,48 @@
   </si>
   <si>
     <t>Próba logowania bez wpisania hasła</t>
+  </si>
+  <si>
+    <t>Register 3</t>
+  </si>
+  <si>
+    <t>Register 4</t>
+  </si>
+  <si>
+    <t>Register 5</t>
+  </si>
+  <si>
+    <t>Register 6</t>
+  </si>
+  <si>
+    <t>Register 7</t>
+  </si>
+  <si>
+    <t>Register 8</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - niepoprawny email</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - za krótkie hasło</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - źle powtórzone hasło</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - brak imienia i nazwiska</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - nie wpisano żadnych danych</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownika - hasło bez wielkiej litery I cyfry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,7 +179,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -397,28 +434,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela3" displayName="Tabela3" ref="A1:E6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Nazwa testu" dataDxfId="11"/>
-    <tableColumn id="2" name="Opis" dataDxfId="10"/>
-    <tableColumn id="3" name="Autor" dataDxfId="9"/>
-    <tableColumn id="4" name="Status" dataDxfId="8"/>
-    <tableColumn id="5" name="Uwagi" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nazwa testu" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Opis" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Autor" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Uwagi" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela38" displayName="Tabela38" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela38" displayName="Tabela38" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Nazwa testu" dataDxfId="4"/>
-    <tableColumn id="2" name="Opis" dataDxfId="3"/>
-    <tableColumn id="3" name="Autor" dataDxfId="2"/>
-    <tableColumn id="4" name="Status" dataDxfId="1"/>
-    <tableColumn id="5" name="Uwagi" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nazwa testu" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Opis" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Autor" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Uwagi" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,7 +723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -802,17 +839,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="52.42578125" customWidth="1"/>
@@ -871,12 +908,105 @@
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>